<commit_message>
Monday 18 December 2023
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -214,6 +214,89 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3545966" cy="575976"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1281588" cy="1173575"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -538,419 +621,420 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A9:M19"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="20" customWidth="1"/>
     <col min="6" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>530375.2399999993</v>
-      </c>
-      <c r="G2">
-        <v>530375.2399999993</v>
-      </c>
-      <c r="H2">
-        <v>187.8600000000009</v>
-      </c>
-      <c r="I2">
-        <v>187.8600000000009</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3">
-        <v>382.80999999999995</v>
-      </c>
-      <c r="G3">
-        <v>382.80999999999995</v>
-      </c>
-      <c r="H3">
-        <v>1001.4400000000023</v>
-      </c>
-      <c r="I3">
-        <v>1001.4400000000023</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4">
-        <v>3.8508879999999532</v>
-      </c>
-      <c r="G4">
-        <v>386.6608879999999</v>
-      </c>
-      <c r="H4">
-        <v>135435</v>
-      </c>
-      <c r="I4">
-        <v>136436.44</v>
-      </c>
-      <c r="J4">
-        <v>1124</v>
-      </c>
-      <c r="K4">
-        <v>1124</v>
-      </c>
-      <c r="L4">
-        <v>257.5106130000001</v>
-      </c>
-      <c r="M4">
-        <v>257.5106130000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5">
-        <v>382.80999999999995</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5">
-        <v>1001.4400000000023</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6">
-        <v>3.8508879999999532</v>
-      </c>
-      <c r="G6">
-        <v>386.6608879999999</v>
-      </c>
-      <c r="H6">
-        <v>135435</v>
-      </c>
-      <c r="I6">
-        <v>136436.44</v>
-      </c>
-      <c r="J6">
-        <v>1124</v>
-      </c>
-      <c r="K6">
-        <v>1124</v>
-      </c>
-      <c r="L6">
-        <v>257.5106130000001</v>
-      </c>
-      <c r="M6">
-        <v>257.5106130000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7">
-        <v>382.80999999999995</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7">
-        <v>1001.4400000000023</v>
-      </c>
-      <c r="I7"/>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8">
-        <v>530375.2399999993</v>
-      </c>
-      <c r="G8">
-        <v>530761.9008879993</v>
-      </c>
-      <c r="H8">
-        <v>187.8600000000009</v>
-      </c>
-      <c r="I8">
-        <v>136624.30000000002</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>1124</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>257.5106130000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9">
-        <v>3.8508879999999532</v>
-      </c>
-      <c r="G9"/>
-      <c r="H9">
-        <v>135435</v>
-      </c>
-      <c r="I9"/>
-      <c r="J9">
-        <v>1124</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9">
-        <v>257.5106130000001</v>
-      </c>
-      <c r="M9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F10">
-        <v>382.80999999999995</v>
-      </c>
-      <c r="G10"/>
+        <v>530375.2399999993</v>
+      </c>
+      <c r="G10">
+        <v>530375.2399999993</v>
+      </c>
       <c r="H10">
-        <v>1001.4400000000023</v>
-      </c>
-      <c r="I10"/>
+        <v>187.8600000000009</v>
+      </c>
+      <c r="I10">
+        <v>187.8600000000009</v>
+      </c>
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10"/>
+      <c r="K10">
+        <v>0</v>
+      </c>
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10"/>
+      <c r="M10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>382.80999999999995</v>
+      </c>
+      <c r="G11">
+        <v>382.80999999999995</v>
+      </c>
+      <c r="H11">
+        <v>1001.4400000000023</v>
+      </c>
+      <c r="I11">
+        <v>1001.4400000000023</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>3.8508879999999532</v>
+      </c>
+      <c r="G12">
+        <v>386.6608879999999</v>
+      </c>
+      <c r="H12">
+        <v>135435</v>
+      </c>
+      <c r="I12">
+        <v>136436.44</v>
+      </c>
+      <c r="J12">
+        <v>1124</v>
+      </c>
+      <c r="K12">
+        <v>1124</v>
+      </c>
+      <c r="L12">
+        <v>257.5106130000001</v>
+      </c>
+      <c r="M12">
+        <v>257.5106130000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <v>382.80999999999995</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13">
+        <v>1001.4400000000023</v>
+      </c>
+      <c r="I13"/>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14">
+        <v>3.8508879999999532</v>
+      </c>
+      <c r="G14">
+        <v>386.6608879999999</v>
+      </c>
+      <c r="H14">
+        <v>135435</v>
+      </c>
+      <c r="I14">
+        <v>136436.44</v>
+      </c>
+      <c r="J14">
+        <v>1124</v>
+      </c>
+      <c r="K14">
+        <v>1124</v>
+      </c>
+      <c r="L14">
+        <v>257.5106130000001</v>
+      </c>
+      <c r="M14">
+        <v>257.5106130000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>382.80999999999995</v>
+      </c>
+      <c r="G15"/>
+      <c r="H15">
+        <v>1001.4400000000023</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15"/>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16">
+        <v>530375.2399999993</v>
+      </c>
+      <c r="G16">
+        <v>530761.9008879993</v>
+      </c>
+      <c r="H16">
+        <v>187.8600000000009</v>
+      </c>
+      <c r="I16">
+        <v>136624.30000000002</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1124</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>257.5106130000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17">
+        <v>3.8508879999999532</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17">
+        <v>135435</v>
+      </c>
+      <c r="I17"/>
+      <c r="J17">
+        <v>1124</v>
+      </c>
+      <c r="K17"/>
+      <c r="L17">
+        <v>257.5106130000001</v>
+      </c>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>382.80999999999995</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18">
+        <v>1001.4400000000023</v>
+      </c>
+      <c r="I18"/>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18"/>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F11">
+      <c r="F19">
         <v>3.8508879999999532</v>
       </c>
-      <c r="G11">
+      <c r="G19">
         <v>3.8508879999999532</v>
       </c>
-      <c r="H11">
+      <c r="H19">
         <v>135435</v>
       </c>
-      <c r="I11">
+      <c r="I19">
         <v>135435</v>
       </c>
-      <c r="J11">
+      <c r="J19">
         <v>1124</v>
       </c>
-      <c r="K11">
+      <c r="K19">
         <v>1124</v>
       </c>
-      <c r="L11">
+      <c r="L19">
         <v>257.5106130000001</v>
       </c>
-      <c r="M11">
+      <c r="M19">
         <v>257.5106130000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="M16:M18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>